<commit_message>
agregado de la modificacion de usuario en la BD, todas las funciones fueron comentadas
</commit_message>
<xml_diff>
--- a/Archivos de trabajo/Informes/Excel/AhoraBien.xlsx
+++ b/Archivos de trabajo/Informes/Excel/AhoraBien.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -604,13 +604,13 @@
         <v>44138</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>44138.33333333334</v>
+        <v>44138.35</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>44138.52083333334</v>
+        <v>44138.52777777778</v>
       </c>
       <c r="G3" s="5" t="n">
-        <v>44138.54166666666</v>
+        <v>44138.55069444444</v>
       </c>
       <c r="H3" s="5" t="n">
         <v>44138.74236111111</v>
@@ -634,13 +634,241 @@
         <v>44138</v>
       </c>
       <c r="O3" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="P3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="n">
         <v>0</v>
       </c>
-      <c r="P3" t="n">
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>52</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SIRAGUSA JAVIER CARLOS S. </t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Miércoles</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>44139</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>44139.32777777778</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>44139.74236111111</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>44139</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <v>44139</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <v>44139</v>
+      </c>
+      <c r="J4" s="5" t="n">
+        <v>44139</v>
+      </c>
+      <c r="K4" s="5" t="n">
+        <v>44139</v>
+      </c>
+      <c r="L4" s="5" t="n">
+        <v>44139</v>
+      </c>
+      <c r="M4" s="5" t="n">
+        <v>44139</v>
+      </c>
+      <c r="N4" s="5" t="n">
+        <v>44139</v>
+      </c>
+      <c r="O4" t="n">
+        <v>8</v>
+      </c>
+      <c r="P4" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="Q4" t="n">
         <v>0</v>
       </c>
-      <c r="Q3" t="n">
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>52</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SIRAGUSA JAVIER CARLOS S. </t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Jueves</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>44140</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>44140.32777777778</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>44140.71527777778</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>44140</v>
+      </c>
+      <c r="H5" s="5" t="n">
+        <v>44140</v>
+      </c>
+      <c r="I5" s="5" t="n">
+        <v>44140</v>
+      </c>
+      <c r="J5" s="5" t="n">
+        <v>44140</v>
+      </c>
+      <c r="K5" s="5" t="n">
+        <v>44140</v>
+      </c>
+      <c r="L5" s="5" t="n">
+        <v>44140</v>
+      </c>
+      <c r="M5" s="5" t="n">
+        <v>44140</v>
+      </c>
+      <c r="N5" s="5" t="n">
+        <v>44140</v>
+      </c>
+      <c r="O5" t="n">
         <v>8</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>52</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SIRAGUSA JAVIER CARLOS S. </t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Viernes</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>44141</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>44141.32569444443</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>44141.52708333332</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>44141.55</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <v>44141.74236111111</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <v>44141</v>
+      </c>
+      <c r="J6" s="5" t="n">
+        <v>44141</v>
+      </c>
+      <c r="K6" s="5" t="n">
+        <v>44141</v>
+      </c>
+      <c r="L6" s="5" t="n">
+        <v>44141</v>
+      </c>
+      <c r="M6" s="5" t="n">
+        <v>44141</v>
+      </c>
+      <c r="N6" s="5" t="n">
+        <v>44141</v>
+      </c>
+      <c r="O6" t="n">
+        <v>8</v>
+      </c>
+      <c r="P6" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>52</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SIRAGUSA JAVIER CARLOS S. </t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Sábado</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>44142</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>44142.32569444443</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>44142.50069444445</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>44142</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>44142</v>
+      </c>
+      <c r="I7" s="5" t="n">
+        <v>44142</v>
+      </c>
+      <c r="J7" s="5" t="n">
+        <v>44142</v>
+      </c>
+      <c r="K7" s="5" t="n">
+        <v>44142</v>
+      </c>
+      <c r="L7" s="5" t="n">
+        <v>44142</v>
+      </c>
+      <c r="M7" s="5" t="n">
+        <v>44142</v>
+      </c>
+      <c r="N7" s="5" t="n">
+        <v>44142</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -704,16 +932,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>39.6</v>
       </c>
       <c r="D2" t="n">
-        <v>1.12</v>
+        <v>4.88</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>